<commit_message>
add references, update packages
</commit_message>
<xml_diff>
--- a/data/packages.xlsx
+++ b/data/packages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\judit\Dropbox\GitHub\r-exploration\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE2CB02-3DC6-42D5-8A9E-A49E88599CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D9CD3F-034C-4BFF-8B93-FAC279536589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2240" yWindow="2240" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
   <si>
     <t>package</t>
   </si>
@@ -238,6 +238,24 @@
   </si>
   <si>
     <t>tidyverse core</t>
+  </si>
+  <si>
+    <t>ggpmisc</t>
+  </si>
+  <si>
+    <t>ggplot2 extension which includes tables</t>
+  </si>
+  <si>
+    <t>gt</t>
+  </si>
+  <si>
+    <t>create tables in R</t>
+  </si>
+  <si>
+    <t>gtextras</t>
+  </si>
+  <si>
+    <t>add-on to gt that lets you add visualizations into tables</t>
   </si>
 </sst>
 </file>
@@ -555,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D12"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -940,6 +958,39 @@
         <v>68</v>
       </c>
     </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update packages and references
</commit_message>
<xml_diff>
--- a/data/packages.xlsx
+++ b/data/packages.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\judit\Dropbox\GitHub\r-exploration\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20115FCE-DA59-498D-9F49-E3AB44FE7FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB9E908-83D3-407B-80E5-E5FF6437A294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="2240" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$E$47</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="114">
   <si>
     <t>package</t>
   </si>
@@ -259,16 +262,134 @@
   </si>
   <si>
     <t>documentation for packages</t>
+  </si>
+  <si>
+    <t>cowplot</t>
+  </si>
+  <si>
+    <t>Streamlined plot theme and plot annotations for ggplot2</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>espnscrapeR</t>
+  </si>
+  <si>
+    <t>https://github.com/jthomasmock/espnscrapeR</t>
+  </si>
+  <si>
+    <t>collect or scrape QBR, NFL standings, and stats from ESPN</t>
+  </si>
+  <si>
+    <t>data import</t>
+  </si>
+  <si>
+    <t>geofacet</t>
+  </si>
+  <si>
+    <t>map</t>
+  </si>
+  <si>
+    <t>geofaceting functionality for ggplot2</t>
+  </si>
+  <si>
+    <t>https://hafen.github.io/geofacet/</t>
+  </si>
+  <si>
+    <t>https://github.com/jbaileyh/geogrid</t>
+  </si>
+  <si>
+    <t>Turn geospatial polygons like states, counties or local authorities into regular or hexagonal grids automatically.</t>
+  </si>
+  <si>
+    <t>geogrid</t>
+  </si>
+  <si>
+    <t>https://www.garrickadenbuie.com/project/ggpomological/</t>
+  </si>
+  <si>
+    <t>ggpomological</t>
+  </si>
+  <si>
+    <t>water-colour look for figures</t>
+  </si>
+  <si>
+    <t>ggspatial</t>
+  </si>
+  <si>
+    <t>https://paleolimbot.github.io/ggspatial/index.html</t>
+  </si>
+  <si>
+    <t>Spatial data plus the power of the ggplot2 framework</t>
+  </si>
+  <si>
+    <t>ggetch</t>
+  </si>
+  <si>
+    <t>https://github.com/ricardo-bion/ggtech</t>
+  </si>
+  <si>
+    <t>Tech themes and scales</t>
+  </si>
+  <si>
+    <t>marketing</t>
+  </si>
+  <si>
+    <t>ggthemes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some extra geoms, scales, and themes for ggplot.
+</t>
+  </si>
+  <si>
+    <t>https://jrnold.github.io/ggthemes/index.html</t>
+  </si>
+  <si>
+    <t>hrbrthemes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional Themes and Theme Components for ‘ggplot2’
+</t>
+  </si>
+  <si>
+    <t>https://cinc.rud.is/web/packages/hrbrthemes/</t>
+  </si>
+  <si>
+    <t>bookdown</t>
+  </si>
+  <si>
+    <t>https://bookdown.org/</t>
+  </si>
+  <si>
+    <t>Write HTML, PDF, ePub, and Kindle books with R Markdown</t>
+  </si>
+  <si>
+    <t>R markdown</t>
+  </si>
+  <si>
+    <t>reproducible thesis</t>
+  </si>
+  <si>
+    <t>reproducible documents</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -291,13 +412,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -576,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -587,7 +714,7 @@
     <col min="1" max="1" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -600,281 +727,344 @@
       <c r="D1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
         <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>90</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>100</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
       </c>
       <c r="D11" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
         <v>41</v>
@@ -883,74 +1073,62 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>113</v>
       </c>
       <c r="C30" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C31" t="s">
-        <v>41</v>
-      </c>
-      <c r="D31" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>41</v>
-      </c>
-      <c r="D32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="D33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -961,51 +1139,176 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="C35" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
-      </c>
-      <c r="C36" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="D36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="D37" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>76</v>
-      </c>
-      <c r="B38" t="s">
-        <v>77</v>
-      </c>
-      <c r="C38" t="s">
-        <v>0</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>29</v>
+      </c>
+      <c r="B45" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>108</v>
+      </c>
+      <c r="B48" t="s">
+        <v>110</v>
+      </c>
+      <c r="C48" t="s">
+        <v>111</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E47" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E47">
+      <sortCondition ref="A1:A47"/>
+    </sortState>
+  </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{2F5432C7-C247-4F56-BC2E-B610C73BDDFE}"/>
+    <hyperlink ref="E7" r:id="rId2" xr:uid="{88F0D0A3-DD2D-4CF8-AA84-B3307BC396D6}"/>
+    <hyperlink ref="E8" r:id="rId3" xr:uid="{39D3B35B-0DC2-4D50-B510-48FF6D3C477B}"/>
+    <hyperlink ref="E13" r:id="rId4" xr:uid="{9EDCDAD9-1C17-4BF2-AA2A-BAFA0E9FC517}"/>
+    <hyperlink ref="E10" r:id="rId5" xr:uid="{FF20A815-C676-4B5D-AFAA-BF2A8EF14C38}"/>
+    <hyperlink ref="E17" r:id="rId6" xr:uid="{EB018138-991E-46A8-90EC-288D1DD2C939}"/>
+    <hyperlink ref="E21" r:id="rId7" xr:uid="{51998BA9-1BD9-41F5-83FD-0AC6B3E64C8E}"/>
+    <hyperlink ref="E48" r:id="rId8" xr:uid="{C75CB427-457B-4C89-B306-0FE984EC6EEA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>